<commit_message>
FS meta data entry
</commit_message>
<xml_diff>
--- a/LabyDivDis_Metadata.xlsx
+++ b/LabyDivDis_Metadata.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1460" yWindow="1060" windowWidth="19960" windowHeight="14940" tabRatio="500"/>
+    <workbookView xWindow="680" yWindow="460" windowWidth="21180" windowHeight="15380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="130407" concurrentCalc="0"/>
+  <calcPr calcId="130407"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,77 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
+  <si>
+    <t>Collected healthy (i.e. lesion free) seagrass leaves from stock seagrass growing in greenhouse</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Scraped off epiphytes</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cut leaves into 270 1 cm segments (Vectors) and distributed vectors across 27 glass vials (VWR 66011-121) filled to 3/4 full with seawater using tweezers (10 leaf segments/vial_</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Covered all vials individually with tinfoil and autoclaved at 121 for 20 minutes</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>Control and disease vector prep continued</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t xml:space="preserve"> (see vector inoculation protocol from T2 for details)</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Control and disease vector check</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shoot inoculation 9am-4pm</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Inoculated control vases FS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Inoculation protocol:</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Clipped vectors directly to leaf tisuse (targetted 2nd leaf 5cm from top of sheath when possible, noted if otherwise) </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shoot inoculation 9am-12pm</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Inoculated disease vases FS, RH, TH</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Inoculation protocol</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Check disease and control shoots for leasions FS, RH</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Checked disease shoots for lesions FS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
   <si>
     <t>Controls vectors: C1-C13 ok</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -128,40 +198,6 @@
       </rPr>
       <t xml:space="preserve"> (see vector inoculation protocol from T2 for details)</t>
     </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Collected healthy (i.e. lesion free) seagrass leaves from stock seagrass growing in greenhouse</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Scraped off epiphytes</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cut leaves into 270 1 cm segments (Vectors) and distributed vectors across 27 glass vials (VWR 66011-121) filled to 3/4 full with seawater using tweezers (10 leaf segments/vial_</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Covered all vials individually with tinfoil and autoclaved at 121 for 20 minutes</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>Control and disease vector prep continued</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t xml:space="preserve"> (see vector inoculation protocol from T2 for details)</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Control and disease vector check</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -549,17 +585,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:G79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F65" sqref="F65"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -569,7 +605,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="C4" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -580,7 +616,7 @@
     <row r="7" spans="1:3">
       <c r="B7" s="1"/>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -594,7 +630,7 @@
     <row r="10" spans="1:3">
       <c r="B10" s="1"/>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -605,7 +641,7 @@
     <row r="13" spans="1:3">
       <c r="B13" s="1"/>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -615,27 +651,27 @@
     </row>
     <row r="16" spans="1:3">
       <c r="C16" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="2:6">
       <c r="D17" t="s">
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:6">
       <c r="D18" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="2:6">
       <c r="D19" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="2:6">
       <c r="D20" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="2:6">
@@ -645,42 +681,42 @@
     </row>
     <row r="23" spans="2:6">
       <c r="C23" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="2:6">
       <c r="D24" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="2:6">
       <c r="E25" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="2:6">
       <c r="E26" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="2:6">
       <c r="F27" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="2:6">
       <c r="F28" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="2:6">
       <c r="D29" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="2:6">
       <c r="E30" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="2:6">
@@ -690,22 +726,22 @@
     </row>
     <row r="33" spans="2:7">
       <c r="C33" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="2:7">
       <c r="D34" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="2:7">
       <c r="D35" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36" spans="2:7">
       <c r="D36" s="2" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
@@ -718,32 +754,32 @@
     </row>
     <row r="39" spans="2:7">
       <c r="C39" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
     </row>
     <row r="40" spans="2:7">
       <c r="C40" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="41" spans="2:7">
       <c r="D41" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
     </row>
     <row r="42" spans="2:7">
       <c r="E42" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
     </row>
     <row r="43" spans="2:7">
       <c r="E43" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
     </row>
     <row r="44" spans="2:7">
       <c r="E44" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
     </row>
     <row r="46" spans="2:7">
@@ -753,66 +789,135 @@
     </row>
     <row r="47" spans="2:7">
       <c r="C47" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="48" spans="2:7">
       <c r="C48" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="50" spans="3:5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5">
       <c r="C50" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="51" spans="3:5">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5">
       <c r="D51" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="52" spans="3:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5">
       <c r="D52" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="53" spans="3:5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5">
       <c r="D53" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="54" spans="3:5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5">
       <c r="D54" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="56" spans="3:5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5">
       <c r="D56" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="57" spans="3:5">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5">
       <c r="E57" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="58" spans="3:5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5">
       <c r="E58" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="60" spans="3:5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5">
       <c r="D60" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="61" spans="3:5">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5">
       <c r="E61" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5">
+      <c r="B63" s="1">
+        <v>41695</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5">
+      <c r="C64" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5">
+      <c r="C65" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5">
+      <c r="D66" t="s">
         <v>8</v>
       </c>
     </row>
+    <row r="67" spans="2:5">
+      <c r="E67" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5">
+      <c r="B69" s="1">
+        <v>41696</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5">
+      <c r="C70" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5">
+      <c r="C71" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5">
+      <c r="D72" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5">
+      <c r="E73" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="75" spans="2:5">
+      <c r="B75" s="1">
+        <v>41702</v>
+      </c>
+    </row>
+    <row r="76" spans="2:5">
+      <c r="C76" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="78" spans="2:5">
+      <c r="B78" s="1">
+        <v>41706</v>
+      </c>
+    </row>
+    <row r="79" spans="2:5">
+      <c r="C79" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
FS DIVDIS 1 month analysis
Diversity by disease analyses
</commit_message>
<xml_diff>
--- a/LabyDivDis_Metadata.xlsx
+++ b/LabyDivDis_Metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="21180" windowHeight="15380" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="21180" windowHeight="15380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Greenhouse" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
   <si>
     <t xml:space="preserve">Clipped vectors directly to leaf tisuse (targetted 2nd leaf 5cm from top of sheath when possible, noted if otherwise) </t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -95,6 +95,10 @@
   </si>
   <si>
     <t>ASU ribbon cut to ~30cm and tied on one end to a small plastic coated paper clip (anchor)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Surveyed seedlings for survival, shoot number, length, and disease presence/absence and lesion size</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -590,17 +594,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:G82"/>
+  <dimension ref="A1:G85"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -656,27 +660,27 @@
     </row>
     <row r="16" spans="1:3">
       <c r="C16" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="2:6">
       <c r="D17" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="2:6">
       <c r="D18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="2:6">
       <c r="D19" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="2:6">
       <c r="D20" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="2:6">
@@ -686,42 +690,42 @@
     </row>
     <row r="23" spans="2:6">
       <c r="C23" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="2:6">
       <c r="D24" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="2:6">
       <c r="E25" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="2:6">
       <c r="E26" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="2:6">
       <c r="F27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="2:6">
       <c r="F28" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="2:6">
       <c r="D29" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="2:6">
       <c r="E30" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="2:6">
@@ -731,7 +735,7 @@
     </row>
     <row r="33" spans="2:7">
       <c r="C33" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="2:7">
@@ -764,7 +768,7 @@
     </row>
     <row r="40" spans="2:7">
       <c r="C40" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="41" spans="2:7">
@@ -779,12 +783,12 @@
     </row>
     <row r="43" spans="2:7">
       <c r="E43" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="44" spans="2:7">
       <c r="E44" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="46" spans="2:7">
@@ -804,47 +808,47 @@
     </row>
     <row r="50" spans="2:5">
       <c r="C50" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="51" spans="2:5">
       <c r="D51" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="52" spans="2:5">
       <c r="D52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="53" spans="2:5">
       <c r="D53" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="54" spans="2:5">
       <c r="D54" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="56" spans="2:5">
       <c r="D56" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="57" spans="2:5">
       <c r="E57" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="58" spans="2:5">
       <c r="E58" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="60" spans="2:5">
       <c r="D60" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="61" spans="2:5">
@@ -859,17 +863,17 @@
     </row>
     <row r="64" spans="2:5">
       <c r="C64" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="65" spans="2:5">
       <c r="C65" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="66" spans="2:5">
       <c r="D66" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="67" spans="2:5">
@@ -929,11 +933,20 @@
     </row>
     <row r="82" spans="2:3">
       <c r="C82" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3">
+      <c r="B84" s="1">
+        <v>41723</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3">
+      <c r="C85" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -948,13 +961,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData/>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
FS edits for 1month post inoculatin Analyses
Shoot number analyses and figures 1month post inoculation for team seagrass
</commit_message>
<xml_diff>
--- a/LabyDivDis_Metadata.xlsx
+++ b/LabyDivDis_Metadata.xlsx
@@ -22,106 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
   <si>
-    <t xml:space="preserve">Clipped vectors directly to leaf tisuse (targetted 2nd leaf 5cm from top of sheath when possible, noted if otherwise) </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Shoot inoculation 9am-12pm</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Inoculated disease vases FS, RH, TH</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Inoculation protocol</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Check disease and control shoots for leasions FS, RH</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Checked disease shoots for lesions FS</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Controls vectors: C1-C13 ok</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Disease vectors: D2, D4, D5, D7-D10, D12-D14 ok</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Desease vectors: D1, D3, D6, D11 contaminated</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Shoots checked for signs of disease (lesions)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>No obvious signs of disease on either control or disease treated plants, decided to re-inoculate with direct clip</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Surveyed seedlings for survival</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Surveyed seedlings for survival and shoot number</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Surveyed seedlings for survival, shoot number, and length</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Labelled FS C1-13 2/20/18 &amp; FS D1-D14 2/20/18</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Shoot inoculation 9am-12pm</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Started supplementary light treatment in Greenhouse. 16 hrs/day (5am-9pm); 99- Red, 99- Blue, 99- White.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Inoculation protocol:</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ASU ribbon cut to ~30cm and tied on one end to a small plastic coated paper clip (anchor)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Surveyed seedlings for survival, shoot number, length, and disease presence/absence and lesion size</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Then 2 vectors clipped to each ribbon using plastic tubing at 10cm and 20cm from paperclip</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ribbons with vectors placed in the middle of each vase (paper cilp side down)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Inoculated control vases first and then inoculated disease vases FS, RH, TCH, MR</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>In hood plated 10 vectors per petri dish on Laby SSA media (27 dishes plated) in a circular formation (~ 3 cm diameter)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Disease vectors plated second</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>After plating disease vectors incoculated the center of the circle of vectors with agar plug cut from the growing edge of Laby Culture T5091417C_3A (isolated from seagrass leaf collected from Dorothy Cove)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -207,6 +107,106 @@
   </si>
   <si>
     <t>Inoculation protocol:</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Clipped vectors directly to leaf tisuse (targetted 2nd leaf 5cm from top of sheath when possible, noted if otherwise) </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shoot inoculation 9am-12pm</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Inoculated disease vases FS, RH, TH</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Inoculation protocol</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Check disease and control shoots for leasions FS, RH</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Checked disease shoots for lesions FS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Controls vectors: C1-C13 ok</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Disease vectors: D2, D4, D5, D7-D10, D12-D14 ok</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Desease vectors: D1, D3, D6, D11 contaminated</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shoots checked for signs of disease (lesions)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>No obvious signs of disease on either control or disease treated plants, decided to re-inoculate with direct clip</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Surveyed seedlings for survival</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Surveyed seedlings for survival and shoot number</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Surveyed seedlings for survival, shoot number, and length</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Labelled FS C1-13 2/20/18 &amp; FS D1-D14 2/20/18</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shoot inoculation 9am-12pm</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Started supplementary light treatment in Greenhouse. 16 hrs/day (5am-9pm); 99- Red, 99- Blue, 99- White.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Inoculation protocol:</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASU ribbon cut to ~30cm and tied on one end to a small plastic coated paper clip (anchor)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Surveyed seedlings for survival, shoot number, length, and disease presence/absence and lesion size</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Then 2 vectors clipped to each ribbon using plastic tubing at 10cm and 20cm from paperclip</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ribbons with vectors placed in the middle of each vase (paper cilp side down)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Inoculated control vases first and then inoculated disease vases FS, RH, TCH, MR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>In hood plated 10 vectors per petri dish on Laby SSA media (27 dishes plated) in a circular formation (~ 3 cm diameter)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Disease vectors plated second</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -596,7 +596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:G85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
       <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
@@ -604,7 +604,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -614,7 +614,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="C4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -625,7 +625,7 @@
     <row r="7" spans="1:3">
       <c r="B7" s="1"/>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -639,7 +639,7 @@
     <row r="10" spans="1:3">
       <c r="B10" s="1"/>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -650,7 +650,7 @@
     <row r="13" spans="1:3">
       <c r="B13" s="1"/>
       <c r="C13" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -660,27 +660,27 @@
     </row>
     <row r="16" spans="1:3">
       <c r="C16" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="2:6">
       <c r="D17" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="2:6">
       <c r="D18" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="2:6">
       <c r="D19" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="2:6">
       <c r="D20" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="2:6">
@@ -690,42 +690,42 @@
     </row>
     <row r="23" spans="2:6">
       <c r="C23" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="2:6">
       <c r="D24" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="2:6">
       <c r="E25" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="2:6">
       <c r="E26" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="2:6">
       <c r="F27" t="s">
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:6">
       <c r="F28" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="2:6">
       <c r="D29" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="2:6">
       <c r="E30" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="2:6">
@@ -735,22 +735,22 @@
     </row>
     <row r="33" spans="2:7">
       <c r="C33" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
     </row>
     <row r="34" spans="2:7">
       <c r="D34" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="2:7">
       <c r="D35" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
     </row>
     <row r="36" spans="2:7">
       <c r="D36" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
@@ -763,32 +763,32 @@
     </row>
     <row r="39" spans="2:7">
       <c r="C39" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="2:7">
       <c r="C40" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="2:7">
       <c r="D41" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
     </row>
     <row r="42" spans="2:7">
       <c r="E42" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="2:7">
       <c r="E43" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
     </row>
     <row r="44" spans="2:7">
       <c r="E44" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="2:7">
@@ -798,62 +798,62 @@
     </row>
     <row r="47" spans="2:7">
       <c r="C47" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
     </row>
     <row r="48" spans="2:7">
       <c r="C48" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
     </row>
     <row r="50" spans="2:5">
       <c r="C50" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
     </row>
     <row r="51" spans="2:5">
       <c r="D51" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
     </row>
     <row r="52" spans="2:5">
       <c r="D52" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
     </row>
     <row r="53" spans="2:5">
       <c r="D53" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54" spans="2:5">
       <c r="D54" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
     </row>
     <row r="56" spans="2:5">
       <c r="D56" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
     </row>
     <row r="57" spans="2:5">
       <c r="E57" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="2:5">
       <c r="E58" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
     </row>
     <row r="60" spans="2:5">
       <c r="D60" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
     </row>
     <row r="61" spans="2:5">
       <c r="E61" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="63" spans="2:5">
@@ -863,22 +863,22 @@
     </row>
     <row r="64" spans="2:5">
       <c r="C64" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
     </row>
     <row r="65" spans="2:5">
       <c r="C65" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
     </row>
     <row r="66" spans="2:5">
       <c r="D66" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
     </row>
     <row r="67" spans="2:5">
       <c r="E67" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
     </row>
     <row r="69" spans="2:5">
@@ -888,22 +888,22 @@
     </row>
     <row r="70" spans="2:5">
       <c r="C70" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
     </row>
     <row r="71" spans="2:5">
       <c r="C71" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="72" spans="2:5">
       <c r="D72" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
     </row>
     <row r="73" spans="2:5">
       <c r="E73" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
     </row>
     <row r="75" spans="2:5">
@@ -913,7 +913,7 @@
     </row>
     <row r="76" spans="2:5">
       <c r="C76" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
     </row>
     <row r="78" spans="2:5">
@@ -923,7 +923,7 @@
     </row>
     <row r="79" spans="2:5">
       <c r="C79" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="81" spans="2:3">
@@ -933,7 +933,7 @@
     </row>
     <row r="82" spans="2:3">
       <c r="C82" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
     </row>
     <row r="84" spans="2:3">
@@ -943,10 +943,11 @@
     </row>
     <row r="85" spans="2:3">
       <c r="C85" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -969,7 +970,6 @@
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>